<commit_message>
remove to-do, change list to copyonwritearraylist, update time-records
</commit_message>
<xml_diff>
--- a/documents/time-records/Fritz Verena_c7031304.xlsx
+++ b/documents/time-records/Fritz Verena_c7031304.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bolia\Documents\erweiterungsstudium\swe\PS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACCAB026-C7D2-4BB7-AF54-68C4243754FE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{196F018B-B249-476D-8C93-0A1937D6AF81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33750" yWindow="3135" windowWidth="21600" windowHeight="11385" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
   </bookViews>
   <sheets>
     <sheet name="Datenerfassung" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="71">
   <si>
     <t>Datum</t>
   </si>
@@ -235,6 +235,21 @@
   </si>
   <si>
     <t>Runde beenden durch Timer</t>
+  </si>
+  <si>
+    <t>Status update, merge requests</t>
+  </si>
+  <si>
+    <t>Absprache issues, merge requests</t>
+  </si>
+  <si>
+    <t>alertMessages für CubeStatus im GameRoom einbauen</t>
+  </si>
+  <si>
+    <t>CubeStatus Messages u. Anzeige</t>
+  </si>
+  <si>
+    <t>Desginentscheidungen, to-dos für Abnahmetest</t>
   </si>
 </sst>
 </file>
@@ -665,7 +680,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C47" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C57" sqref="C57"/>
+      <selection pane="bottomRight" activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1481,29 +1496,74 @@
       </c>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="5"/>
-      <c r="B59" s="6"/>
-      <c r="D59" s="8"/>
+      <c r="A59" s="5">
+        <v>44324</v>
+      </c>
+      <c r="B59" s="6">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D59" s="8" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="60" spans="1:4">
-      <c r="A60" s="5"/>
-      <c r="B60" s="6"/>
-      <c r="D60" s="8"/>
+      <c r="A60" s="5">
+        <v>44327</v>
+      </c>
+      <c r="B60" s="6">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="61" spans="1:4">
-      <c r="A61" s="5"/>
-      <c r="B61" s="6"/>
-      <c r="D61" s="8"/>
-    </row>
-    <row r="62" spans="1:4">
-      <c r="A62" s="5"/>
-      <c r="B62" s="6"/>
-      <c r="D62" s="8"/>
-    </row>
-    <row r="63" spans="1:4">
-      <c r="A63" s="5"/>
-      <c r="B63" s="6"/>
-      <c r="D63" s="8"/>
+      <c r="A61" s="5">
+        <v>44328</v>
+      </c>
+      <c r="B61" s="6">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D61" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="31.5">
+      <c r="A62" s="5">
+        <v>44329</v>
+      </c>
+      <c r="B62" s="6">
+        <v>0.125</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D62" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="31.5">
+      <c r="A63" s="5">
+        <v>44329</v>
+      </c>
+      <c r="B63" s="6">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D63" s="8" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="5"/>

</xml_diff>

<commit_message>
fix and update time-records
</commit_message>
<xml_diff>
--- a/documents/time-records/Fritz Verena_c7031304.xlsx
+++ b/documents/time-records/Fritz Verena_c7031304.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bolia\Documents\erweiterungsstudium\swe\PS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E5E7D1C-7501-4BD9-BC80-9ECA67CFD1ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{403C39D2-593F-4FEB-A124-27FB20D37953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
   </bookViews>
   <sheets>
     <sheet name="Datenerfassung" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="82">
   <si>
     <t>Datum</t>
   </si>
@@ -271,6 +271,18 @@
   </si>
   <si>
     <t>bug fixes</t>
+  </si>
+  <si>
+    <t>check merge requests, fix tests</t>
+  </si>
+  <si>
+    <t>bug fix, merge requests</t>
+  </si>
+  <si>
+    <t>solve merge requests</t>
+  </si>
+  <si>
+    <t>Besprechung Abschlussbericht</t>
   </si>
 </sst>
 </file>
@@ -714,25 +726,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F855F84B-A166-7442-8B83-EBB2C6A67214}">
-  <dimension ref="A1:D1004"/>
+  <dimension ref="A1:D1003"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C56" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C63" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D68" sqref="D68"/>
+      <selection pane="bottomRight" activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="10.625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="9.625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="37.75" style="7" customWidth="1"/>
-    <col min="4" max="4" width="38.25" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.59765625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="9.59765625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="37.69921875" style="7" customWidth="1"/>
+    <col min="4" max="4" width="38.19921875" style="10" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="11" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" ht="31.5">
+    <row r="1" spans="1:4" s="4" customFormat="1" ht="31.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -942,7 +954,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="31.5">
+    <row r="16" spans="1:4" ht="31.2">
       <c r="A16" s="5">
         <v>44279</v>
       </c>
@@ -1024,7 +1036,7 @@
       </c>
       <c r="D21" s="8"/>
     </row>
-    <row r="22" spans="1:4" ht="31.5">
+    <row r="22" spans="1:4" ht="31.2">
       <c r="A22" s="5">
         <v>44287</v>
       </c>
@@ -1066,7 +1078,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="31.5">
+    <row r="25" spans="1:4" ht="31.2">
       <c r="A25" s="5">
         <v>44292</v>
       </c>
@@ -1152,40 +1164,47 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="5">
-        <v>44299</v>
-      </c>
-      <c r="B31" s="6"/>
-      <c r="D31" s="8"/>
+        <v>44300</v>
+      </c>
+      <c r="B31" s="6">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="5">
         <v>44300</v>
       </c>
       <c r="B32" s="6">
-        <v>4.1666666666666664E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="31.2">
       <c r="A33" s="5">
-        <v>44300</v>
+        <v>44303</v>
       </c>
       <c r="B33" s="6">
-        <v>2.0833333333333332E-2</v>
+        <v>0.10416666666666667</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="31.5">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" s="5">
         <v>44303</v>
       </c>
@@ -1196,12 +1215,12 @@
         <v>5</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="5">
-        <v>44303</v>
+        <v>44304</v>
       </c>
       <c r="B35" s="6">
         <v>0.10416666666666667</v>
@@ -1210,35 +1229,35 @@
         <v>5</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="5">
-        <v>44304</v>
+        <v>44305</v>
       </c>
       <c r="B36" s="6">
-        <v>0.10416666666666667</v>
+        <v>0.125</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="5">
-        <v>44305</v>
+        <v>44306</v>
       </c>
       <c r="B37" s="6">
-        <v>0.125</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1246,35 +1265,35 @@
         <v>44306</v>
       </c>
       <c r="B38" s="6">
-        <v>8.3333333333333329E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="5">
-        <v>44306</v>
+        <v>44307</v>
       </c>
       <c r="B39" s="6">
-        <v>6.25E-2</v>
+        <v>4.3750000000000004E-2</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="5">
-        <v>44307</v>
+        <v>44308</v>
       </c>
       <c r="B40" s="6">
-        <v>4.3750000000000004E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="C40" s="7" t="s">
         <v>5</v>
@@ -1285,10 +1304,10 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="5">
-        <v>44308</v>
+        <v>44311</v>
       </c>
       <c r="B41" s="6">
-        <v>4.1666666666666664E-2</v>
+        <v>0.10416666666666667</v>
       </c>
       <c r="C41" s="7" t="s">
         <v>5</v>
@@ -1302,18 +1321,18 @@
         <v>44311</v>
       </c>
       <c r="B42" s="6">
-        <v>0.10416666666666667</v>
+        <v>6.25E-2</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="5">
-        <v>44311</v>
+        <v>44313</v>
       </c>
       <c r="B43" s="6">
         <v>6.25E-2</v>
@@ -1322,7 +1341,7 @@
         <v>14</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1330,18 +1349,18 @@
         <v>44313</v>
       </c>
       <c r="B44" s="6">
-        <v>6.25E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="5">
-        <v>44313</v>
+        <v>44314</v>
       </c>
       <c r="B45" s="6">
         <v>4.1666666666666664E-2</v>
@@ -1350,49 +1369,49 @@
         <v>5</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="5">
-        <v>44314</v>
+        <v>44315</v>
       </c>
       <c r="B46" s="6">
-        <v>4.1666666666666664E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="C46" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="5">
-        <v>44315</v>
+        <v>44317</v>
       </c>
       <c r="B47" s="6">
-        <v>6.25E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="5">
-        <v>44317</v>
+        <v>44318</v>
       </c>
       <c r="B48" s="6">
-        <v>2.0833333333333332E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1406,7 +1425,7 @@
         <v>5</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1417,38 +1436,38 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="5">
-        <v>44318</v>
+        <v>44319</v>
       </c>
       <c r="B51" s="6">
-        <v>4.1666666666666664E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="5">
-        <v>44319</v>
+        <v>44320</v>
       </c>
       <c r="B52" s="6">
-        <v>8.3333333333333329E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1456,18 +1475,18 @@
         <v>44320</v>
       </c>
       <c r="B53" s="6">
-        <v>4.1666666666666664E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="5">
-        <v>44320</v>
+        <v>44321</v>
       </c>
       <c r="B54" s="6">
         <v>8.3333333333333329E-2</v>
@@ -1476,7 +1495,7 @@
         <v>5</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -1487,57 +1506,57 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="5">
-        <v>44321</v>
+        <v>44322</v>
       </c>
       <c r="B56" s="6">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="5">
-        <v>44322</v>
+        <v>44323</v>
       </c>
       <c r="B57" s="6">
-        <v>8.3333333333333329E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="5">
-        <v>44323</v>
+        <v>44324</v>
       </c>
       <c r="B58" s="6">
-        <v>6.25E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="5">
-        <v>44324</v>
+        <v>44327</v>
       </c>
       <c r="B59" s="6">
         <v>4.1666666666666664E-2</v>
@@ -1546,182 +1565,218 @@
         <v>14</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="5">
-        <v>44327</v>
+        <v>44328</v>
       </c>
       <c r="B60" s="6">
-        <v>4.1666666666666664E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="C60" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="31.2">
+      <c r="A61" s="5">
+        <v>44329</v>
+      </c>
+      <c r="B61" s="6">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C61" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D60" s="8" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
-      <c r="A61" s="5">
-        <v>44328</v>
-      </c>
-      <c r="B61" s="6">
-        <v>6.25E-2</v>
-      </c>
-      <c r="C61" s="7" t="s">
-        <v>11</v>
-      </c>
       <c r="D61" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="31.5">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="31.2">
       <c r="A62" s="5">
         <v>44329</v>
       </c>
       <c r="B62" s="6">
-        <v>8.3333333333333329E-2</v>
+        <v>0.10416666666666667</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" ht="31.5">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
       <c r="A63" s="5">
         <v>44329</v>
       </c>
       <c r="B63" s="6">
-        <v>0.10416666666666667</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="5">
-        <v>44329</v>
+        <v>44333</v>
       </c>
       <c r="B64" s="6">
-        <v>0.16666666666666666</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="5">
-        <v>44333</v>
-      </c>
-      <c r="B65" s="6">
-        <v>4.1666666666666664E-2</v>
+        <v>44334</v>
+      </c>
+      <c r="B65" s="12">
+        <v>6.25E-2</v>
       </c>
       <c r="C65" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D65" s="8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4">
+      <c r="D65" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="31.2">
       <c r="A66" s="5">
-        <v>44334</v>
-      </c>
-      <c r="B66" s="12">
-        <v>6.25E-2</v>
+        <v>44335</v>
+      </c>
+      <c r="B66" s="6">
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="C66" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D66" s="11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" ht="31.5">
+      <c r="D66" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="46.8">
       <c r="A67" s="5">
-        <v>44335</v>
+        <v>44336</v>
       </c>
       <c r="B67" s="6">
-        <v>8.3333333333333329E-2</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="C67" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="47.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
       <c r="A68" s="5">
-        <v>44336</v>
+        <v>44343</v>
       </c>
       <c r="B68" s="6">
-        <v>0.16666666666666666</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="5">
-        <v>44343</v>
+        <v>44345</v>
       </c>
       <c r="B69" s="6">
-        <v>4.1666666666666664E-2</v>
+        <v>0.125</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="5">
-        <v>44345</v>
+        <v>44346</v>
       </c>
       <c r="B70" s="6">
-        <v>0.125</v>
+        <v>6.25E-2</v>
       </c>
       <c r="C70" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="71" spans="1:4">
-      <c r="A71" s="5"/>
-      <c r="B71" s="6"/>
-      <c r="D71" s="8"/>
+      <c r="A71" s="5">
+        <v>44347</v>
+      </c>
+      <c r="B71" s="6">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D71" s="8" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="72" spans="1:4">
-      <c r="A72" s="5"/>
-      <c r="B72" s="6"/>
-      <c r="D72" s="8"/>
+      <c r="A72" s="5">
+        <v>44348</v>
+      </c>
+      <c r="B72" s="6">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D72" s="8" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="73" spans="1:4">
-      <c r="A73" s="5"/>
-      <c r="B73" s="6"/>
-      <c r="D73" s="8"/>
+      <c r="A73" s="5">
+        <v>44353</v>
+      </c>
+      <c r="B73" s="6">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D73" s="8" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="74" spans="1:4">
-      <c r="A74" s="5"/>
-      <c r="B74" s="6"/>
-      <c r="D74" s="8"/>
+      <c r="A74" s="5">
+        <v>44356</v>
+      </c>
+      <c r="B74" s="6">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D74" s="8" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="5"/>
@@ -6364,12 +6419,7 @@
       <c r="D1002" s="8"/>
     </row>
     <row r="1003" spans="1:4">
-      <c r="A1003" s="5"/>
-      <c r="B1003" s="6"/>
-      <c r="D1003" s="8"/>
-    </row>
-    <row r="1004" spans="1:4">
-      <c r="A1004" s="9"/>
+      <c r="A1003" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -6381,7 +6431,7 @@
           <x14:formula1>
             <xm:f>Tätigkeiten!$B$2:$B$12</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C1003</xm:sqref>
+          <xm:sqref>C2:C1002</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -6395,9 +6445,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
-    <col min="2" max="2" width="34.625" customWidth="1"/>
+    <col min="2" max="2" width="34.59765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">

</xml_diff>